<commit_message>
Added filling stand with items, having a item info of items in a stand, gold usage, update usage of build area, being able to set extra permission to build different things in different areas.
</commit_message>
<xml_diff>
--- a/Shopper_2d/CSV/building.xlsx
+++ b/Shopper_2d/CSV/building.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\GodotProjects\Shopper_2d\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C8B66A-0D9F-4621-B119-1DDE9C9AEEE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFF07D1-D155-4DFA-BBA4-68759F2F1E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{6613D835-19EA-40EE-98A1-1D2837994A45}"/>
+    <workbookView xWindow="25490" yWindow="3460" windowWidth="19420" windowHeight="10560" xr2:uid="{6613D835-19EA-40EE-98A1-1D2837994A45}"/>
   </bookViews>
   <sheets>
     <sheet name="shop_item" sheetId="1" r:id="rId1"/>
@@ -76,16 +76,16 @@
     <t>sprite_path</t>
   </si>
   <si>
-    <t>res://Asset/shelf.png</t>
-  </si>
-  <si>
-    <t>res://Asset/stand.png</t>
-  </si>
-  <si>
-    <t>res://Asset/hang.png</t>
-  </si>
-  <si>
     <t>unlocked</t>
+  </si>
+  <si>
+    <t>res://Asset/Building/shelf.png</t>
+  </si>
+  <si>
+    <t>res://Asset/Building/stand.png</t>
+  </si>
+  <si>
+    <t>res://Asset/Building/hang.png</t>
   </si>
 </sst>
 </file>
@@ -934,7 +934,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,7 +942,7 @@
     <col min="4" max="4" width="20.85546875" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" customWidth="1"/>
     <col min="6" max="6" width="22.7109375" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.28515625" customWidth="1"/>
   </cols>
@@ -964,7 +964,7 @@
         <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -981,7 +981,7 @@
         <v>300</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1001,7 +1001,7 @@
         <v>250</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1021,7 +1021,7 @@
         <v>200</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4">
         <v>1</v>

</xml_diff>